<commit_message>
added wing,drum and thigh gen
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/marel/recap_marel.xlsx
+++ b/CustomLabelPrinter/src/paperwork/marel/recap_marel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\marel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81A47F4-1381-4258-89C5-3D8BF083348B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277DD41B-BD48-49A0-A656-5C78D911E4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="1305" windowWidth="25665" windowHeight="15975" activeTab="5" xr2:uid="{9D1CC91B-B205-4EC5-83C4-0AB214C674BC}"/>
+    <workbookView xWindow="4695" yWindow="1155" windowWidth="25665" windowHeight="15975" activeTab="1" xr2:uid="{9D1CC91B-B205-4EC5-83C4-0AB214C674BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Thigh" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
   <si>
     <t>PRODUCTION RECAP SHEET</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>Production Output</t>
+  </si>
+  <si>
+    <t>WOGS</t>
+  </si>
+  <si>
+    <t>LEG 1/4</t>
   </si>
 </sst>
 </file>
@@ -415,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -465,39 +471,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1175,7 +1148,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -1192,7 +1165,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1213,38 +1186,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1264,49 +1237,49 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1336,28 +1309,65 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1369,214 +1379,175 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2049,7 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699CEC77-1DDB-44EC-B40A-4D63677C0CA6}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2600,8 +2571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156580C-15A5-42B9-984B-1C692F9D4B57}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2988,123 +2959,123 @@
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
+      <c r="A26" s="87">
+        <v>17756</v>
+      </c>
+      <c r="B26" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="151"/>
+      <c r="D26" s="151"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="151"/>
+      <c r="G26" s="151"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="151"/>
+      <c r="K26" s="151"/>
+      <c r="L26" s="151"/>
+      <c r="M26" s="89"/>
     </row>
     <row r="27" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
+      <c r="A27" s="87">
+        <v>10453</v>
+      </c>
+      <c r="B27" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="151"/>
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="89"/>
     </row>
     <row r="28" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
     </row>
     <row r="29" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="73">
-        <v>22258</v>
-      </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="77"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="75"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="77"/>
+      <c r="A30" s="86"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="73">
-        <v>21102</v>
-      </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="77"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75">
-        <v>22486</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="77"/>
+      <c r="A32" s="86"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="1">
     <mergeCell ref="A28:M28"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="A31:B32"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M31:M32"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -3116,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C1F370-9287-40D1-B25E-87CA9C1B0C97}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3541,17 +3512,17 @@
       <c r="C28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="78"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="79"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="92"/>
       <c r="H28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="79"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="92"/>
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -3564,17 +3535,17 @@
       <c r="C29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="78"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="92"/>
       <c r="H29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="78"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="79"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="92"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="92"/>
       <c r="M29" s="16"/>
     </row>
     <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -3649,7 +3620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74483EF0-F135-478D-A883-6A9F25469A97}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3669,11 +3640,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="3" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="17"/>
@@ -3681,11 +3652,11 @@
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
     </row>
     <row r="5" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="18"/>
@@ -3735,82 +3706,82 @@
       <c r="A10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="124"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="73"/>
     </row>
     <row r="11" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="124"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
     </row>
     <row r="12" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="124"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
     </row>
     <row r="13" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="124"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
     </row>
     <row r="14" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="73"/>
     </row>
     <row r="15" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="73"/>
     </row>
     <row r="16" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="124"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
     </row>
     <row r="17" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="124"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="73"/>
     </row>
     <row r="18" spans="1:5" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="125"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="126"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="75"/>
     </row>
     <row r="19" spans="1:5" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
@@ -3819,28 +3790,28 @@
       <c r="A20" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="127"/>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="128"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
     </row>
     <row r="21" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="73"/>
     </row>
     <row r="22" spans="1:5" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="125"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="126"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="75"/>
     </row>
     <row r="23" spans="1:5" ht="29.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
@@ -3913,22 +3884,22 @@
     </row>
     <row r="2" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="J3" s="110" t="s">
+      <c r="B3" s="111"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="J3" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="110"/>
-      <c r="L3" s="113" t="s">
+      <c r="K3" s="111"/>
+      <c r="L3" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="113"/>
+      <c r="M3" s="121"/>
     </row>
     <row r="4" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3942,33 +3913,33 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="111" t="s">
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104" t="s">
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="104"/>
-      <c r="P7" s="104" t="s">
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="104"/>
-      <c r="R7" s="104"/>
-      <c r="S7" s="112"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="115"/>
     </row>
     <row r="8" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
@@ -3976,116 +3947,116 @@
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
-      <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
-      <c r="Q8" s="129"/>
-      <c r="R8" s="129"/>
-      <c r="S8" s="130"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="118"/>
+      <c r="R8" s="118"/>
+      <c r="S8" s="119"/>
     </row>
     <row r="9" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="131"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="131"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="132"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="103"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="103"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="103"/>
+      <c r="S9" s="104"/>
     </row>
     <row r="10" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="132"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="103"/>
+      <c r="O10" s="103"/>
+      <c r="P10" s="103"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="104"/>
     </row>
     <row r="11" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="131"/>
-      <c r="M11" s="131"/>
-      <c r="N11" s="131"/>
-      <c r="O11" s="131"/>
-      <c r="P11" s="131"/>
-      <c r="Q11" s="131"/>
-      <c r="R11" s="131"/>
-      <c r="S11" s="132"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="104"/>
     </row>
     <row r="12" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
-      <c r="N12" s="133"/>
-      <c r="O12" s="133"/>
-      <c r="P12" s="133"/>
-      <c r="Q12" s="133"/>
-      <c r="R12" s="133"/>
-      <c r="S12" s="134"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="106"/>
+      <c r="K12" s="106"/>
+      <c r="L12" s="106"/>
+      <c r="M12" s="106"/>
+      <c r="N12" s="106"/>
+      <c r="O12" s="106"/>
+      <c r="P12" s="106"/>
+      <c r="Q12" s="106"/>
+      <c r="R12" s="106"/>
+      <c r="S12" s="107"/>
     </row>
     <row r="13" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -4093,116 +4064,116 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
-      <c r="S13" s="130"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="118"/>
+      <c r="S13" s="119"/>
     </row>
     <row r="14" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="88" t="s">
+      <c r="D14" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="131"/>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="131"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="131"/>
-      <c r="O14" s="131"/>
-      <c r="P14" s="131"/>
-      <c r="Q14" s="131"/>
-      <c r="R14" s="131"/>
-      <c r="S14" s="132"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="103"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="104"/>
     </row>
     <row r="15" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="131"/>
-      <c r="O15" s="131"/>
-      <c r="P15" s="131"/>
-      <c r="Q15" s="131"/>
-      <c r="R15" s="131"/>
-      <c r="S15" s="132"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="103"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="103"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="103"/>
+      <c r="O15" s="103"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="103"/>
+      <c r="S15" s="104"/>
     </row>
     <row r="16" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="88" t="s">
+      <c r="D16" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="131"/>
-      <c r="O16" s="131"/>
-      <c r="P16" s="131"/>
-      <c r="Q16" s="131"/>
-      <c r="R16" s="131"/>
-      <c r="S16" s="132"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="103"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="103"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="103"/>
+      <c r="O16" s="103"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="103"/>
+      <c r="S16" s="104"/>
     </row>
     <row r="17" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="114" t="s">
+      <c r="D17" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="135"/>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
-      <c r="O17" s="137"/>
-      <c r="P17" s="135"/>
-      <c r="Q17" s="136"/>
-      <c r="R17" s="136"/>
-      <c r="S17" s="138"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="96"/>
+      <c r="S17" s="97"/>
     </row>
     <row r="18" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
@@ -4210,70 +4181,70 @@
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="105" t="s">
+      <c r="D18" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="131"/>
-      <c r="I18" s="131"/>
-      <c r="J18" s="131"/>
-      <c r="K18" s="131"/>
-      <c r="L18" s="139"/>
-      <c r="M18" s="139"/>
-      <c r="N18" s="139"/>
-      <c r="O18" s="139"/>
-      <c r="P18" s="139"/>
-      <c r="Q18" s="139"/>
-      <c r="R18" s="139"/>
-      <c r="S18" s="140"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="103"/>
+      <c r="J18" s="103"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="109"/>
+      <c r="O18" s="109"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="109"/>
+      <c r="R18" s="109"/>
+      <c r="S18" s="110"/>
     </row>
     <row r="19" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="131"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="131"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="131"/>
-      <c r="O19" s="131"/>
-      <c r="P19" s="131"/>
-      <c r="Q19" s="131"/>
-      <c r="R19" s="131"/>
-      <c r="S19" s="132"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="103"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="103"/>
+      <c r="Q19" s="103"/>
+      <c r="R19" s="103"/>
+      <c r="S19" s="104"/>
     </row>
     <row r="20" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="133"/>
-      <c r="L20" s="133"/>
-      <c r="M20" s="133"/>
-      <c r="N20" s="133"/>
-      <c r="O20" s="133"/>
-      <c r="P20" s="133"/>
-      <c r="Q20" s="133"/>
-      <c r="R20" s="133"/>
-      <c r="S20" s="134"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="106"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="106"/>
+      <c r="M20" s="106"/>
+      <c r="N20" s="106"/>
+      <c r="O20" s="106"/>
+      <c r="P20" s="106"/>
+      <c r="Q20" s="106"/>
+      <c r="R20" s="106"/>
+      <c r="S20" s="107"/>
     </row>
     <row r="21" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
@@ -4281,93 +4252,93 @@
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="129"/>
-      <c r="I21" s="129"/>
-      <c r="J21" s="129"/>
-      <c r="K21" s="129"/>
-      <c r="L21" s="139"/>
-      <c r="M21" s="139"/>
-      <c r="N21" s="139"/>
-      <c r="O21" s="139"/>
-      <c r="P21" s="139"/>
-      <c r="Q21" s="139"/>
-      <c r="R21" s="139"/>
-      <c r="S21" s="140"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="109"/>
+      <c r="N21" s="109"/>
+      <c r="O21" s="109"/>
+      <c r="P21" s="109"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="110"/>
     </row>
     <row r="22" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="131"/>
-      <c r="I22" s="131"/>
-      <c r="J22" s="131"/>
-      <c r="K22" s="131"/>
-      <c r="L22" s="131"/>
-      <c r="M22" s="131"/>
-      <c r="N22" s="131"/>
-      <c r="O22" s="131"/>
-      <c r="P22" s="131"/>
-      <c r="Q22" s="131"/>
-      <c r="R22" s="131"/>
-      <c r="S22" s="132"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="103"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="103"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="103"/>
+      <c r="M22" s="103"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="103"/>
+      <c r="P22" s="103"/>
+      <c r="Q22" s="103"/>
+      <c r="R22" s="103"/>
+      <c r="S22" s="104"/>
     </row>
     <row r="23" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="131"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131"/>
-      <c r="R23" s="131"/>
-      <c r="S23" s="132"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="103"/>
+      <c r="K23" s="103"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="103"/>
+      <c r="O23" s="103"/>
+      <c r="P23" s="103"/>
+      <c r="Q23" s="103"/>
+      <c r="R23" s="103"/>
+      <c r="S23" s="104"/>
     </row>
     <row r="24" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27"/>
-      <c r="D24" s="93" t="s">
+      <c r="D24" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="133"/>
-      <c r="M24" s="133"/>
-      <c r="N24" s="133"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
-      <c r="Q24" s="133"/>
-      <c r="R24" s="133"/>
-      <c r="S24" s="134"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="106"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="106"/>
+      <c r="K24" s="106"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="106"/>
+      <c r="N24" s="106"/>
+      <c r="O24" s="106"/>
+      <c r="P24" s="106"/>
+      <c r="Q24" s="106"/>
+      <c r="R24" s="106"/>
+      <c r="S24" s="107"/>
     </row>
     <row r="26" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
@@ -4380,172 +4351,275 @@
       </c>
     </row>
     <row r="28" spans="1:19" s="31" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="103" t="s">
+      <c r="A28" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="104"/>
-      <c r="C28" s="104"/>
-      <c r="D28" s="106" t="s">
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="108" t="s">
+      <c r="E28" s="124"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="124"/>
+      <c r="I28" s="124"/>
+      <c r="J28" s="124"/>
+      <c r="K28" s="124"/>
+      <c r="L28" s="124"/>
+      <c r="M28" s="124"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="109"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="126"/>
     </row>
     <row r="29" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="98" t="s">
+      <c r="A29" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="97"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="101"/>
-      <c r="R29" s="101"/>
-      <c r="S29" s="102"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="132"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="132"/>
+      <c r="K29" s="132"/>
+      <c r="L29" s="132"/>
+      <c r="M29" s="132"/>
+      <c r="N29" s="132"/>
+      <c r="O29" s="133"/>
+      <c r="P29" s="134"/>
+      <c r="Q29" s="135"/>
+      <c r="R29" s="135"/>
+      <c r="S29" s="136"/>
     </row>
     <row r="30" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="90"/>
-      <c r="O30" s="91"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="83"/>
-      <c r="R30" s="83"/>
-      <c r="S30" s="84"/>
+      <c r="B30" s="102"/>
+      <c r="C30" s="102"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="127"/>
+      <c r="J30" s="127"/>
+      <c r="K30" s="127"/>
+      <c r="L30" s="127"/>
+      <c r="M30" s="127"/>
+      <c r="N30" s="127"/>
+      <c r="O30" s="128"/>
+      <c r="P30" s="129"/>
+      <c r="Q30" s="130"/>
+      <c r="R30" s="130"/>
+      <c r="S30" s="131"/>
     </row>
     <row r="31" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="88" t="s">
+      <c r="A31" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="89"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="90"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="90"/>
-      <c r="O31" s="91"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="83"/>
-      <c r="R31" s="83"/>
-      <c r="S31" s="84"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="127"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
+      <c r="G31" s="127"/>
+      <c r="H31" s="127"/>
+      <c r="I31" s="127"/>
+      <c r="J31" s="127"/>
+      <c r="K31" s="127"/>
+      <c r="L31" s="127"/>
+      <c r="M31" s="127"/>
+      <c r="N31" s="127"/>
+      <c r="O31" s="128"/>
+      <c r="P31" s="129"/>
+      <c r="Q31" s="130"/>
+      <c r="R31" s="130"/>
+      <c r="S31" s="131"/>
     </row>
     <row r="32" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="90"/>
-      <c r="O32" s="91"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="83"/>
-      <c r="R32" s="83"/>
-      <c r="S32" s="84"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="127"/>
+      <c r="I32" s="127"/>
+      <c r="J32" s="127"/>
+      <c r="K32" s="127"/>
+      <c r="L32" s="127"/>
+      <c r="M32" s="127"/>
+      <c r="N32" s="127"/>
+      <c r="O32" s="128"/>
+      <c r="P32" s="129"/>
+      <c r="Q32" s="130"/>
+      <c r="R32" s="130"/>
+      <c r="S32" s="131"/>
     </row>
     <row r="33" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="90"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="90"/>
-      <c r="O33" s="91"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="83"/>
-      <c r="R33" s="83"/>
-      <c r="S33" s="84"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="127"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="127"/>
+      <c r="J33" s="127"/>
+      <c r="K33" s="127"/>
+      <c r="L33" s="127"/>
+      <c r="M33" s="127"/>
+      <c r="N33" s="127"/>
+      <c r="O33" s="128"/>
+      <c r="P33" s="129"/>
+      <c r="Q33" s="130"/>
+      <c r="R33" s="130"/>
+      <c r="S33" s="131"/>
     </row>
     <row r="34" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="92" t="s">
+      <c r="A34" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="93"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="94"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="85"/>
-      <c r="Q34" s="86"/>
-      <c r="R34" s="86"/>
-      <c r="S34" s="87"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="140"/>
+      <c r="I34" s="140"/>
+      <c r="J34" s="140"/>
+      <c r="K34" s="140"/>
+      <c r="L34" s="140"/>
+      <c r="M34" s="140"/>
+      <c r="N34" s="140"/>
+      <c r="O34" s="141"/>
+      <c r="P34" s="137"/>
+      <c r="Q34" s="138"/>
+      <c r="R34" s="138"/>
+      <c r="S34" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="127">
+    <mergeCell ref="P33:S33"/>
+    <mergeCell ref="P34:S34"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:S32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:S31"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="P30:S30"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="P24:S24"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="P28:S28"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P15:S15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="P13:S13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="C3:F3"/>
     <mergeCell ref="P17:S17"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="H17:K17"/>
@@ -4570,109 +4644,6 @@
     <mergeCell ref="L18:O18"/>
     <mergeCell ref="P18:S18"/>
     <mergeCell ref="D19:G19"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="P13:S13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P15:S15"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="P24:S24"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="P28:S28"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:S31"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P29:S29"/>
-    <mergeCell ref="P30:S30"/>
-    <mergeCell ref="P33:S33"/>
-    <mergeCell ref="P34:S34"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="P32:S32"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -4684,7 +4655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581AB293-5767-4BF6-9DCC-8977856CE4E1}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D30" sqref="D30:F30"/>
     </sheetView>
   </sheetViews>
@@ -4741,11 +4712,11 @@
       <c r="C4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
       <c r="G4" s="53" t="s">
         <v>79</v>
       </c>
@@ -4786,496 +4757,496 @@
     <row r="5" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
-      <c r="H5" s="141"/>
-      <c r="I5" s="141"/>
-      <c r="J5" s="141"/>
-      <c r="K5" s="141"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="141"/>
-      <c r="N5" s="141"/>
-      <c r="O5" s="141"/>
-      <c r="P5" s="141"/>
-      <c r="Q5" s="141"/>
-      <c r="R5" s="142"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
     </row>
     <row r="6" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="46"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="143"/>
-      <c r="K6" s="143"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="143"/>
-      <c r="P6" s="143"/>
-      <c r="Q6" s="143"/>
-      <c r="R6" s="144"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="81"/>
     </row>
     <row r="7" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="46"/>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="143"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="144"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="81"/>
     </row>
     <row r="8" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="46"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="143"/>
-      <c r="K8" s="143"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="143"/>
-      <c r="N8" s="143"/>
-      <c r="O8" s="143"/>
-      <c r="P8" s="143"/>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="144"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="81"/>
     </row>
     <row r="9" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="46"/>
-      <c r="C9" s="143"/>
-      <c r="D9" s="143"/>
-      <c r="E9" s="143"/>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="143"/>
-      <c r="I9" s="143"/>
-      <c r="J9" s="143"/>
-      <c r="K9" s="143"/>
-      <c r="L9" s="143"/>
-      <c r="M9" s="143"/>
-      <c r="N9" s="143"/>
-      <c r="O9" s="143"/>
-      <c r="P9" s="143"/>
-      <c r="Q9" s="143"/>
-      <c r="R9" s="144"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="81"/>
     </row>
     <row r="10" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="46"/>
-      <c r="C10" s="143"/>
-      <c r="D10" s="143"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="143"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="143"/>
-      <c r="K10" s="143"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="143"/>
-      <c r="N10" s="143"/>
-      <c r="O10" s="143"/>
-      <c r="P10" s="143"/>
-      <c r="Q10" s="143"/>
-      <c r="R10" s="144"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="81"/>
     </row>
     <row r="11" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
       <c r="B11" s="46"/>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="143"/>
-      <c r="F11" s="143"/>
-      <c r="G11" s="143"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="143"/>
-      <c r="L11" s="143"/>
-      <c r="M11" s="143"/>
-      <c r="N11" s="143"/>
-      <c r="O11" s="143"/>
-      <c r="P11" s="143"/>
-      <c r="Q11" s="143"/>
-      <c r="R11" s="144"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="81"/>
     </row>
     <row r="12" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45"/>
       <c r="B12" s="46"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="143"/>
-      <c r="E12" s="143"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="143"/>
-      <c r="I12" s="143"/>
-      <c r="J12" s="143"/>
-      <c r="K12" s="143"/>
-      <c r="L12" s="143"/>
-      <c r="M12" s="143"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="143"/>
-      <c r="P12" s="143"/>
-      <c r="Q12" s="143"/>
-      <c r="R12" s="144"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="81"/>
     </row>
     <row r="13" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45"/>
       <c r="B13" s="46"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
-      <c r="F13" s="143"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="143"/>
-      <c r="M13" s="143"/>
-      <c r="N13" s="143"/>
-      <c r="O13" s="143"/>
-      <c r="P13" s="143"/>
-      <c r="Q13" s="143"/>
-      <c r="R13" s="144"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="81"/>
     </row>
     <row r="14" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
       <c r="B14" s="46"/>
-      <c r="C14" s="143"/>
-      <c r="D14" s="143"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="143"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="143"/>
-      <c r="I14" s="143"/>
-      <c r="J14" s="143"/>
-      <c r="K14" s="143"/>
-      <c r="L14" s="143"/>
-      <c r="M14" s="143"/>
-      <c r="N14" s="143"/>
-      <c r="O14" s="143"/>
-      <c r="P14" s="143"/>
-      <c r="Q14" s="143"/>
-      <c r="R14" s="144"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="81"/>
     </row>
     <row r="15" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
       <c r="B15" s="46"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="143"/>
-      <c r="F15" s="143"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="143"/>
-      <c r="I15" s="143"/>
-      <c r="J15" s="143"/>
-      <c r="K15" s="143"/>
-      <c r="L15" s="143"/>
-      <c r="M15" s="143"/>
-      <c r="N15" s="143"/>
-      <c r="O15" s="143"/>
-      <c r="P15" s="143"/>
-      <c r="Q15" s="143"/>
-      <c r="R15" s="144"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="81"/>
     </row>
     <row r="16" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
       <c r="B16" s="46"/>
-      <c r="C16" s="143"/>
-      <c r="D16" s="143"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="143"/>
-      <c r="G16" s="143"/>
-      <c r="H16" s="143"/>
-      <c r="I16" s="143"/>
-      <c r="J16" s="143"/>
-      <c r="K16" s="143"/>
-      <c r="L16" s="143"/>
-      <c r="M16" s="143"/>
-      <c r="N16" s="143"/>
-      <c r="O16" s="143"/>
-      <c r="P16" s="143"/>
-      <c r="Q16" s="143"/>
-      <c r="R16" s="144"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
     </row>
     <row r="17" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
       <c r="B17" s="46"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="143"/>
-      <c r="E17" s="143"/>
-      <c r="F17" s="143"/>
-      <c r="G17" s="143"/>
-      <c r="H17" s="143"/>
-      <c r="I17" s="143"/>
-      <c r="J17" s="143"/>
-      <c r="K17" s="143"/>
-      <c r="L17" s="143"/>
-      <c r="M17" s="143"/>
-      <c r="N17" s="143"/>
-      <c r="O17" s="143"/>
-      <c r="P17" s="143"/>
-      <c r="Q17" s="143"/>
-      <c r="R17" s="144"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
     </row>
     <row r="18" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
       <c r="B18" s="46"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="143"/>
-      <c r="P18" s="143"/>
-      <c r="Q18" s="143"/>
-      <c r="R18" s="144"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="81"/>
     </row>
     <row r="19" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
       <c r="B19" s="46"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="143"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="143"/>
-      <c r="M19" s="143"/>
-      <c r="N19" s="143"/>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="144"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="81"/>
     </row>
     <row r="20" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="45"/>
       <c r="B20" s="46"/>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="143"/>
-      <c r="L20" s="143"/>
-      <c r="M20" s="143"/>
-      <c r="N20" s="143"/>
-      <c r="O20" s="143"/>
-      <c r="P20" s="143"/>
-      <c r="Q20" s="143"/>
-      <c r="R20" s="144"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="81"/>
     </row>
     <row r="21" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45"/>
       <c r="B21" s="46"/>
-      <c r="C21" s="143"/>
-      <c r="D21" s="143"/>
-      <c r="E21" s="143"/>
-      <c r="F21" s="143"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="143"/>
-      <c r="I21" s="143"/>
-      <c r="J21" s="143"/>
-      <c r="K21" s="143"/>
-      <c r="L21" s="143"/>
-      <c r="M21" s="143"/>
-      <c r="N21" s="143"/>
-      <c r="O21" s="143"/>
-      <c r="P21" s="143"/>
-      <c r="Q21" s="143"/>
-      <c r="R21" s="144"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="81"/>
     </row>
     <row r="22" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
-      <c r="E22" s="143"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="143"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="143"/>
-      <c r="J22" s="143"/>
-      <c r="K22" s="143"/>
-      <c r="L22" s="143"/>
-      <c r="M22" s="143"/>
-      <c r="N22" s="143"/>
-      <c r="O22" s="143"/>
-      <c r="P22" s="143"/>
-      <c r="Q22" s="143"/>
-      <c r="R22" s="144"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="81"/>
     </row>
     <row r="23" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
       <c r="B23" s="46"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="143"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="143"/>
-      <c r="J23" s="143"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="143"/>
-      <c r="O23" s="143"/>
-      <c r="P23" s="143"/>
-      <c r="Q23" s="143"/>
-      <c r="R23" s="144"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="81"/>
     </row>
     <row r="24" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="143"/>
-      <c r="E24" s="143"/>
-      <c r="F24" s="143"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="143"/>
-      <c r="J24" s="143"/>
-      <c r="K24" s="143"/>
-      <c r="L24" s="143"/>
-      <c r="M24" s="143"/>
-      <c r="N24" s="143"/>
-      <c r="O24" s="143"/>
-      <c r="P24" s="143"/>
-      <c r="Q24" s="143"/>
-      <c r="R24" s="144"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="81"/>
     </row>
     <row r="25" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="46"/>
-      <c r="C25" s="143"/>
-      <c r="D25" s="143"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="143"/>
-      <c r="J25" s="143"/>
-      <c r="K25" s="143"/>
-      <c r="L25" s="143"/>
-      <c r="M25" s="143"/>
-      <c r="N25" s="143"/>
-      <c r="O25" s="143"/>
-      <c r="P25" s="143"/>
-      <c r="Q25" s="143"/>
-      <c r="R25" s="144"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="80"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="81"/>
     </row>
     <row r="26" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="46"/>
-      <c r="C26" s="143"/>
-      <c r="D26" s="143"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="143"/>
-      <c r="I26" s="143"/>
-      <c r="J26" s="143"/>
-      <c r="K26" s="143"/>
-      <c r="L26" s="143"/>
-      <c r="M26" s="143"/>
-      <c r="N26" s="143"/>
-      <c r="O26" s="143"/>
-      <c r="P26" s="143"/>
-      <c r="Q26" s="143"/>
-      <c r="R26" s="144"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="81"/>
     </row>
     <row r="27" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="46"/>
-      <c r="C27" s="143"/>
-      <c r="D27" s="143"/>
-      <c r="E27" s="143"/>
-      <c r="F27" s="143"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="143"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="143"/>
-      <c r="K27" s="143"/>
-      <c r="L27" s="143"/>
-      <c r="M27" s="143"/>
-      <c r="N27" s="143"/>
-      <c r="O27" s="143"/>
-      <c r="P27" s="143"/>
-      <c r="Q27" s="143"/>
-      <c r="R27" s="144"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="80"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="81"/>
     </row>
     <row r="28" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47"/>
       <c r="B28" s="48"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="145"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
-      <c r="K28" s="145"/>
-      <c r="L28" s="145"/>
-      <c r="M28" s="145"/>
-      <c r="N28" s="145"/>
-      <c r="O28" s="145"/>
-      <c r="P28" s="145"/>
-      <c r="Q28" s="145"/>
-      <c r="R28" s="146"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="83"/>
     </row>
     <row r="29" spans="1:18" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="142" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="118"/>
+      <c r="B29" s="143"/>
       <c r="C29" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="122" t="s">
+      <c r="D29" s="150" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
       <c r="G29" s="49" t="s">
         <v>79</v>
       </c>
@@ -5314,24 +5285,24 @@
       </c>
     </row>
     <row r="30" spans="1:18" s="37" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="119"/>
-      <c r="B30" s="120"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="148"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="147"/>
-      <c r="H30" s="147"/>
-      <c r="I30" s="147"/>
-      <c r="J30" s="147"/>
-      <c r="K30" s="147"/>
-      <c r="L30" s="147"/>
-      <c r="M30" s="147"/>
-      <c r="N30" s="147"/>
-      <c r="O30" s="147"/>
-      <c r="P30" s="147"/>
-      <c r="Q30" s="147"/>
-      <c r="R30" s="151"/>
+      <c r="A30" s="144"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="147"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="149"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="84"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="84"/>
+      <c r="N30" s="84"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="84"/>
+      <c r="Q30" s="84"/>
+      <c r="R30" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
added total for rework
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/marel/recap_marel.xlsx
+++ b/CustomLabelPrinter/src/paperwork/marel/recap_marel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\marel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\marel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277DD41B-BD48-49A0-A656-5C78D911E4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1100845C-3CED-4825-9FDD-56FB0C892473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="1155" windowWidth="25665" windowHeight="15975" activeTab="1" xr2:uid="{9D1CC91B-B205-4EC5-83C4-0AB214C674BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{9D1CC91B-B205-4EC5-83C4-0AB214C674BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Thigh" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
   <si>
     <t>PRODUCTION RECAP SHEET</t>
   </si>
@@ -281,13 +284,16 @@
   </si>
   <si>
     <t>LEG 1/4</t>
+  </si>
+  <si>
+    <t>Drumsticks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1364,6 +1370,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1379,6 +1388,81 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1400,154 +1484,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1635,64 +1641,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
 </file>
 
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2021,19 +1969,19 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="8" customWidth="1"/>
-    <col min="3" max="12" width="5.7109375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="5.75" style="8" customWidth="1"/>
+    <col min="13" max="13" width="18.25" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -2050,19 +1998,24 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="21" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="137" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
       <c r="L2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="63"/>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="21" customHeight="1">
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
@@ -2077,7 +2030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="23.1" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="69"/>
       <c r="C4" s="37"/>
@@ -2092,7 +2045,7 @@
       <c r="L4" s="37"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="23.1" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="69"/>
       <c r="C5" s="37"/>
@@ -2107,7 +2060,7 @@
       <c r="L5" s="37"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="23.1" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="69"/>
       <c r="C6" s="37"/>
@@ -2122,7 +2075,7 @@
       <c r="L6" s="37"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="23.1" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="69"/>
       <c r="C7" s="37"/>
@@ -2137,7 +2090,7 @@
       <c r="L7" s="37"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="23.1" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="69"/>
       <c r="C8" s="37"/>
@@ -2152,7 +2105,7 @@
       <c r="L8" s="37"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="23.1" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="69"/>
       <c r="C9" s="37"/>
@@ -2167,7 +2120,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="23.1" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="69"/>
       <c r="C10" s="37"/>
@@ -2182,7 +2135,7 @@
       <c r="L10" s="37"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="23.1" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="69"/>
       <c r="C11" s="37"/>
@@ -2197,7 +2150,7 @@
       <c r="L11" s="37"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="21" customHeight="1">
       <c r="A12" s="36" t="s">
         <v>59</v>
       </c>
@@ -2214,7 +2167,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="23.1" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="69"/>
       <c r="C13" s="37"/>
@@ -2228,7 +2181,7 @@
       <c r="K13" s="37"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="23.1" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="69"/>
       <c r="C14" s="37"/>
@@ -2242,7 +2195,7 @@
       <c r="K14" s="37"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="23.1" customHeight="1">
       <c r="A15" s="70"/>
       <c r="B15" s="69"/>
       <c r="C15" s="37"/>
@@ -2256,7 +2209,7 @@
       <c r="K15" s="37"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="23.1" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="69"/>
       <c r="C16" s="37"/>
@@ -2270,7 +2223,7 @@
       <c r="K16" s="37"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="23.1" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="69"/>
       <c r="C17" s="37"/>
@@ -2284,7 +2237,7 @@
       <c r="K17" s="37"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="23.1" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="69"/>
       <c r="C18" s="37"/>
@@ -2298,7 +2251,7 @@
       <c r="K18" s="37"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="23.1" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="69"/>
       <c r="C19" s="37"/>
@@ -2312,7 +2265,7 @@
       <c r="K19" s="37"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="23.1" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="69"/>
       <c r="C20" s="37"/>
@@ -2326,7 +2279,7 @@
       <c r="K20" s="37"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="23.1" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="69"/>
       <c r="C21" s="37"/>
@@ -2340,7 +2293,7 @@
       <c r="K21" s="37"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="23.1" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="69"/>
       <c r="C22" s="37"/>
@@ -2354,7 +2307,7 @@
       <c r="K22" s="37"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="23.1" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="69"/>
       <c r="C23" s="37"/>
@@ -2368,7 +2321,7 @@
       <c r="K23" s="37"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="23.1" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="69"/>
       <c r="C24" s="37"/>
@@ -2382,7 +2335,7 @@
       <c r="K24" s="37"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="23.1" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="69"/>
       <c r="C25" s="37"/>
@@ -2396,7 +2349,7 @@
       <c r="K25" s="37"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="23.1" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="69"/>
       <c r="C26" s="37"/>
@@ -2410,7 +2363,7 @@
       <c r="K26" s="37"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="23.1" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="69"/>
       <c r="C27" s="37"/>
@@ -2424,7 +2377,7 @@
       <c r="K27" s="37"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="23.1" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="69"/>
       <c r="C28" s="37"/>
@@ -2438,7 +2391,7 @@
       <c r="K28" s="37"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="23.1" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="69"/>
       <c r="C29" s="37"/>
@@ -2452,7 +2405,7 @@
       <c r="K29" s="37"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="23.1" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="69"/>
       <c r="C30" s="37"/>
@@ -2466,7 +2419,7 @@
       <c r="K30" s="37"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="21" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="69"/>
       <c r="C31" s="37"/>
@@ -2480,7 +2433,7 @@
       <c r="K31" s="37"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="21" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="69"/>
       <c r="C32" s="37"/>
@@ -2494,7 +2447,7 @@
       <c r="K32" s="37"/>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:11" ht="21" customHeight="1">
       <c r="C33" s="37"/>
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
@@ -2505,7 +2458,7 @@
       <c r="J33" s="37"/>
       <c r="K33" s="37"/>
     </row>
-    <row r="34" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:11" ht="21" customHeight="1">
       <c r="C34" s="37"/>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
@@ -2516,7 +2469,7 @@
       <c r="J34" s="37"/>
       <c r="K34" s="37"/>
     </row>
-    <row r="35" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:11" ht="21" customHeight="1">
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
@@ -2527,7 +2480,7 @@
       <c r="J35" s="37"/>
       <c r="K35" s="37"/>
     </row>
-    <row r="36" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:11" ht="21" customHeight="1">
       <c r="C36" s="37"/>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
@@ -2538,7 +2491,7 @@
       <c r="J36" s="37"/>
       <c r="K36" s="37"/>
     </row>
-    <row r="37" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:11" ht="21" customHeight="1">
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
       <c r="E37" s="37"/>
@@ -2549,7 +2502,7 @@
       <c r="J37" s="37"/>
       <c r="K37" s="37"/>
     </row>
-    <row r="38" spans="3:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:11" ht="21" customHeight="1">
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
@@ -2561,6 +2514,9 @@
       <c r="K38" s="37"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -2571,20 +2527,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E156580C-15A5-42B9-984B-1C692F9D4B57}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="8" customWidth="1"/>
-    <col min="3" max="12" width="5.7109375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="5.75" style="8" customWidth="1"/>
+    <col min="13" max="13" width="18.25" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -2601,19 +2557,24 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="21" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="63" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="137" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
       <c r="L2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="63"/>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="21" customHeight="1">
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
@@ -2628,7 +2589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="23.1" customHeight="1">
       <c r="A4" s="70"/>
       <c r="B4" s="69"/>
       <c r="C4" s="37"/>
@@ -2643,7 +2604,7 @@
       <c r="L4" s="37"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="23.1" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="69"/>
       <c r="C5" s="37"/>
@@ -2658,7 +2619,7 @@
       <c r="L5" s="37"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="23.1" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="69"/>
       <c r="C6" s="37"/>
@@ -2673,7 +2634,7 @@
       <c r="L6" s="37"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="23.1" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="69"/>
       <c r="C7" s="37"/>
@@ -2688,7 +2649,7 @@
       <c r="L7" s="37"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="23.1" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="69"/>
       <c r="C8" s="37"/>
@@ -2703,7 +2664,7 @@
       <c r="L8" s="37"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="23.1" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="69"/>
       <c r="C9" s="37"/>
@@ -2718,7 +2679,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="23.1" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="69"/>
       <c r="C10" s="37"/>
@@ -2733,7 +2694,7 @@
       <c r="L10" s="37"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="23.1" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="69"/>
       <c r="C11" s="37"/>
@@ -2748,7 +2709,7 @@
       <c r="L11" s="37"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="23.1" customHeight="1">
       <c r="A12" s="70"/>
       <c r="B12" s="69"/>
       <c r="C12" s="37"/>
@@ -2763,7 +2724,7 @@
       <c r="L12" s="37"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="23.1" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="69"/>
       <c r="C13" s="37"/>
@@ -2778,7 +2739,7 @@
       <c r="L13" s="37"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="23.1" customHeight="1">
       <c r="A14" s="70"/>
       <c r="B14" s="69"/>
       <c r="C14" s="37"/>
@@ -2793,7 +2754,7 @@
       <c r="L14" s="37"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="23.1" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="69"/>
       <c r="C15" s="37"/>
@@ -2808,7 +2769,7 @@
       <c r="L15" s="37"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="23.1" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="69"/>
       <c r="C16" s="37"/>
@@ -2823,7 +2784,7 @@
       <c r="L16" s="37"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="23.1" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="69"/>
       <c r="C17" s="37"/>
@@ -2838,7 +2799,7 @@
       <c r="L17" s="37"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="23.1" customHeight="1">
       <c r="A18" s="70"/>
       <c r="B18" s="69"/>
       <c r="C18" s="37"/>
@@ -2853,7 +2814,7 @@
       <c r="L18" s="37"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="23.1" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="69"/>
       <c r="C19" s="37"/>
@@ -2868,7 +2829,7 @@
       <c r="L19" s="37"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="23.1" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="69"/>
       <c r="C20" s="37"/>
@@ -2883,7 +2844,7 @@
       <c r="L20" s="37"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="23.1" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="69"/>
       <c r="C21" s="37"/>
@@ -2898,7 +2859,7 @@
       <c r="L21" s="37"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="23.1" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="69"/>
       <c r="C22" s="37"/>
@@ -2913,7 +2874,7 @@
       <c r="L22" s="37"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="23.1" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="69"/>
       <c r="C23" s="37"/>
@@ -2928,7 +2889,7 @@
       <c r="L23" s="37"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="23.1" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="69"/>
       <c r="C24" s="37"/>
@@ -2943,7 +2904,7 @@
       <c r="L24" s="37"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="23.1" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="69"/>
       <c r="C25" s="37"/>
@@ -2958,62 +2919,62 @@
       <c r="L25" s="37"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="23.1" customHeight="1">
       <c r="A26" s="87">
         <v>17756</v>
       </c>
       <c r="B26" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="151"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="151"/>
-      <c r="F26" s="151"/>
-      <c r="G26" s="151"/>
-      <c r="H26" s="151"/>
-      <c r="I26" s="151"/>
-      <c r="J26" s="151"/>
-      <c r="K26" s="151"/>
-      <c r="L26" s="151"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
       <c r="M26" s="89"/>
     </row>
-    <row r="27" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="23.1" customHeight="1">
       <c r="A27" s="87">
         <v>10453</v>
       </c>
       <c r="B27" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="151"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="151"/>
-      <c r="H27" s="151"/>
-      <c r="I27" s="151"/>
-      <c r="J27" s="151"/>
-      <c r="K27" s="151"/>
-      <c r="L27" s="151"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
       <c r="M27" s="89"/>
     </row>
-    <row r="28" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="90" t="s">
+    <row r="28" spans="1:13" ht="23.1" customHeight="1">
+      <c r="A28" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-    </row>
-    <row r="29" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="91"/>
+    </row>
+    <row r="29" spans="1:13" ht="23.1" customHeight="1">
       <c r="A29" s="86"/>
       <c r="B29" s="86"/>
       <c r="C29" s="37"/>
@@ -3028,7 +2989,7 @@
       <c r="L29" s="37"/>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="23.1" customHeight="1">
       <c r="A30" s="86"/>
       <c r="B30" s="86"/>
       <c r="C30" s="37"/>
@@ -3043,7 +3004,7 @@
       <c r="L30" s="37"/>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="21" customHeight="1">
       <c r="A31" s="86"/>
       <c r="B31" s="86"/>
       <c r="C31" s="37"/>
@@ -3058,7 +3019,7 @@
       <c r="L31" s="37"/>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="21" customHeight="1">
       <c r="A32" s="86"/>
       <c r="B32" s="86"/>
       <c r="C32" s="37"/>
@@ -3074,8 +3035,9 @@
       <c r="M32" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A28:M28"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -3087,20 +3049,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C1F370-9287-40D1-B25E-87CA9C1B0C97}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="8" customWidth="1"/>
-    <col min="3" max="12" width="5.7109375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="5.75" style="8" customWidth="1"/>
+    <col min="13" max="13" width="18.25" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -3117,19 +3079,24 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="21" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="62" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="137" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
       <c r="L2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="63"/>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="21" customHeight="1">
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
@@ -3144,7 +3111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="23.1" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="69"/>
       <c r="C4" s="37"/>
@@ -3159,7 +3126,7 @@
       <c r="L4" s="37"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="23.1" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="69"/>
       <c r="C5" s="37"/>
@@ -3174,7 +3141,7 @@
       <c r="L5" s="37"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="23.1" customHeight="1">
       <c r="A6" s="70"/>
       <c r="B6" s="69"/>
       <c r="C6" s="37"/>
@@ -3189,7 +3156,7 @@
       <c r="L6" s="37"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="23.1" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="69"/>
       <c r="C7" s="37"/>
@@ -3204,7 +3171,7 @@
       <c r="L7" s="37"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="23.1" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="69"/>
       <c r="C8" s="37"/>
@@ -3219,7 +3186,7 @@
       <c r="L8" s="37"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="23.1" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="69"/>
       <c r="C9" s="37"/>
@@ -3234,7 +3201,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="23.1" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="69"/>
       <c r="C10" s="37"/>
@@ -3249,7 +3216,7 @@
       <c r="L10" s="37"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="23.1" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="69"/>
       <c r="C11" s="37"/>
@@ -3264,7 +3231,7 @@
       <c r="L11" s="37"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="23.1" customHeight="1">
       <c r="A12" s="70"/>
       <c r="B12" s="69"/>
       <c r="C12" s="37"/>
@@ -3279,7 +3246,7 @@
       <c r="L12" s="37"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="23.1" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="69"/>
       <c r="C13" s="37"/>
@@ -3294,7 +3261,7 @@
       <c r="L13" s="37"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="23.1" customHeight="1">
       <c r="A14" s="70"/>
       <c r="B14" s="69"/>
       <c r="C14" s="37"/>
@@ -3309,7 +3276,7 @@
       <c r="L14" s="37"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="23.1" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="69"/>
       <c r="C15" s="37"/>
@@ -3324,7 +3291,7 @@
       <c r="L15" s="37"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="23.1" customHeight="1">
       <c r="A16" s="70"/>
       <c r="B16" s="69"/>
       <c r="C16" s="37"/>
@@ -3339,7 +3306,7 @@
       <c r="L16" s="37"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="23.1" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="69"/>
       <c r="C17" s="37"/>
@@ -3354,7 +3321,7 @@
       <c r="L17" s="37"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="23.1" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="69"/>
       <c r="C18" s="37"/>
@@ -3369,7 +3336,7 @@
       <c r="L18" s="37"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="23.1" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="69"/>
       <c r="C19" s="37"/>
@@ -3384,7 +3351,7 @@
       <c r="L19" s="37"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="23.1" customHeight="1">
       <c r="A20" s="70"/>
       <c r="B20" s="69"/>
       <c r="C20" s="37"/>
@@ -3399,7 +3366,7 @@
       <c r="L20" s="37"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="23.1" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="69"/>
       <c r="C21" s="37"/>
@@ -3414,7 +3381,7 @@
       <c r="L21" s="37"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="23.1" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="69"/>
       <c r="C22" s="37"/>
@@ -3429,7 +3396,7 @@
       <c r="L22" s="37"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="23.1" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="69"/>
       <c r="C23" s="37"/>
@@ -3444,7 +3411,7 @@
       <c r="L23" s="37"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="23.1" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="69"/>
       <c r="C24" s="37"/>
@@ -3459,7 +3426,7 @@
       <c r="L24" s="37"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="23.1" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="69"/>
       <c r="C25" s="37"/>
@@ -3474,7 +3441,7 @@
       <c r="L25" s="37"/>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="23.1" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="69"/>
       <c r="C26" s="37"/>
@@ -3489,7 +3456,7 @@
       <c r="L26" s="37"/>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="23.1" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="69"/>
       <c r="C27" s="37"/>
@@ -3504,7 +3471,7 @@
       <c r="L27" s="37"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="23.1" customHeight="1">
       <c r="A28" s="71"/>
       <c r="B28" s="14" t="s">
         <v>10</v>
@@ -3512,20 +3479,20 @@
       <c r="C28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="91"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="93"/>
       <c r="H28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="91"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="92"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="93"/>
       <c r="M28" s="16"/>
     </row>
-    <row r="29" spans="1:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="23.1" customHeight="1">
       <c r="A29" s="33">
         <v>21301</v>
       </c>
@@ -3535,20 +3502,20 @@
       <c r="C29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="91"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="92"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="93"/>
       <c r="H29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="91"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="93"/>
       <c r="M29" s="16"/>
     </row>
-    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="21" customHeight="1">
       <c r="A30" s="13" t="s">
         <v>8</v>
       </c>
@@ -3565,7 +3532,7 @@
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="21" customHeight="1">
       <c r="A31" s="13" t="s">
         <v>9</v>
       </c>
@@ -3582,7 +3549,7 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="21" customHeight="1">
       <c r="A32" s="13" t="s">
         <v>7</v>
       </c>
@@ -3600,7 +3567,8 @@
       <c r="M32" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="K29:L29"/>
@@ -3624,46 +3592,46 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="27.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
-    <col min="2" max="4" width="17.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="8" customWidth="1"/>
-    <col min="6" max="10" width="15.7109375" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="19.25" style="8" customWidth="1"/>
+    <col min="2" max="4" width="17.75" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.25" style="8" customWidth="1"/>
+    <col min="6" max="10" width="15.75" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="55.5" customHeight="1">
       <c r="B1"/>
       <c r="E1" s="64" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="93" t="s">
+    <row r="2" spans="1:5" ht="29.1" customHeight="1">
+      <c r="B2" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-    </row>
-    <row r="3" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+    </row>
+    <row r="3" spans="1:5" ht="29.1" customHeight="1">
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="94" t="s">
+    <row r="4" spans="1:5" ht="29.1" customHeight="1">
+      <c r="B4" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-    </row>
-    <row r="5" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+    </row>
+    <row r="5" spans="1:5" ht="29.1" customHeight="1">
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="29.1" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3673,8 +3641,8 @@
       </c>
       <c r="E6" s="67"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:5" ht="29.1" customHeight="1" thickBot="1">
       <c r="B8" s="19" t="s">
         <v>20</v>
       </c>
@@ -3685,7 +3653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="32.1" customHeight="1" thickTop="1">
       <c r="A9" s="56" t="s">
         <v>16</v>
       </c>
@@ -3702,7 +3670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="32.1" customHeight="1">
       <c r="A10" s="20" t="s">
         <v>77</v>
       </c>
@@ -3711,7 +3679,7 @@
       <c r="D10" s="72"/>
       <c r="E10" s="73"/>
     </row>
-    <row r="11" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="32.1" customHeight="1">
       <c r="A11" s="20" t="s">
         <v>78</v>
       </c>
@@ -3720,7 +3688,7 @@
       <c r="D11" s="72"/>
       <c r="E11" s="73"/>
     </row>
-    <row r="12" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="32.1" customHeight="1">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -3729,7 +3697,7 @@
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
     </row>
-    <row r="13" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="32.1" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>61</v>
       </c>
@@ -3738,7 +3706,7 @@
       <c r="D13" s="72"/>
       <c r="E13" s="73"/>
     </row>
-    <row r="14" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="32.1" customHeight="1">
       <c r="A14" s="35" t="s">
         <v>23</v>
       </c>
@@ -3747,7 +3715,7 @@
       <c r="D14" s="72"/>
       <c r="E14" s="73"/>
     </row>
-    <row r="15" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="32.1" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>26</v>
       </c>
@@ -3756,7 +3724,7 @@
       <c r="D15" s="72"/>
       <c r="E15" s="73"/>
     </row>
-    <row r="16" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="32.1" customHeight="1">
       <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
@@ -3765,7 +3733,7 @@
       <c r="D16" s="72"/>
       <c r="E16" s="73"/>
     </row>
-    <row r="17" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="32.1" customHeight="1">
       <c r="A17" s="20" t="s">
         <v>28</v>
       </c>
@@ -3774,7 +3742,7 @@
       <c r="D17" s="72"/>
       <c r="E17" s="73"/>
     </row>
-    <row r="18" spans="1:5" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="32.1" customHeight="1" thickBot="1">
       <c r="A18" s="21" t="s">
         <v>29</v>
       </c>
@@ -3783,10 +3751,10 @@
       <c r="D18" s="74"/>
       <c r="E18" s="75"/>
     </row>
-    <row r="19" spans="1:5" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="29.1" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:5" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="32.1" customHeight="1" thickTop="1">
       <c r="A20" s="59" t="s">
         <v>30</v>
       </c>
@@ -3795,7 +3763,7 @@
       <c r="D20" s="76"/>
       <c r="E20" s="77"/>
     </row>
-    <row r="21" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="32.1" customHeight="1">
       <c r="A21" s="60" t="s">
         <v>27</v>
       </c>
@@ -3804,7 +3772,7 @@
       <c r="D21" s="72"/>
       <c r="E21" s="73"/>
     </row>
-    <row r="22" spans="1:5" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="32.1" customHeight="1" thickBot="1">
       <c r="A22" s="61" t="s">
         <v>25</v>
       </c>
@@ -3813,25 +3781,25 @@
       <c r="D22" s="74"/>
       <c r="E22" s="75"/>
     </row>
-    <row r="23" spans="1:5" ht="29.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="29.1" customHeight="1" thickTop="1">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="29.1" customHeight="1">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="29.1" customHeight="1">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="29.1" customHeight="1">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="27.75" customHeight="1">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="27.75" customHeight="1">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="27.75" customHeight="1">
       <c r="A29" s="10"/>
     </row>
   </sheetData>
@@ -3850,16 +3818,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92B5DDE-2A8D-4CB6-8E25-2B1619C4249A}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:O14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.25" defaultRowHeight="21.95" customHeight="1"/>
   <cols>
-    <col min="1" max="16384" width="5.28515625" style="2"/>
+    <col min="1" max="16384" width="5.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="21.95" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>32</v>
       </c>
@@ -3882,641 +3850,744 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+    <row r="2" spans="1:19" ht="12.95" customHeight="1"/>
+    <row r="3" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A3" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="J3" s="111" t="s">
+      <c r="B3" s="117"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="J3" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="111"/>
-      <c r="L3" s="121" t="s">
+      <c r="K3" s="117"/>
+      <c r="L3" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="121"/>
-    </row>
-    <row r="4" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="120"/>
+    </row>
+    <row r="4" spans="1:19" ht="12.95" customHeight="1"/>
+    <row r="5" spans="1:19" ht="21.95" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="112" t="s">
+    <row r="7" spans="1:19" ht="35.1" customHeight="1" thickBot="1">
+      <c r="A7" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="114" t="s">
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113" t="s">
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="113"/>
-      <c r="N7" s="113"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="113" t="s">
+      <c r="M7" s="105"/>
+      <c r="N7" s="105"/>
+      <c r="O7" s="105"/>
+      <c r="P7" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="113"/>
-      <c r="R7" s="113"/>
-      <c r="S7" s="115"/>
-    </row>
-    <row r="8" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="105"/>
+      <c r="R7" s="105"/>
+      <c r="S7" s="119"/>
+    </row>
+    <row r="8" spans="1:19" ht="21.95" customHeight="1">
       <c r="A8" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
-      <c r="D8" s="116" t="s">
+      <c r="D8" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="117"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="117"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="118"/>
-      <c r="K8" s="118"/>
-      <c r="L8" s="118"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="118"/>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="118"/>
-      <c r="S8" s="119"/>
-    </row>
-    <row r="9" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="116"/>
+    </row>
+    <row r="9" spans="1:19" ht="21.95" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-      <c r="Q9" s="103"/>
-      <c r="R9" s="103"/>
-      <c r="S9" s="104"/>
-    </row>
-    <row r="10" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114"/>
+      <c r="R9" s="114"/>
+      <c r="S9" s="115"/>
+    </row>
+    <row r="10" spans="1:19" ht="21.95" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="103"/>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="103"/>
-      <c r="Q10" s="103"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="104"/>
-    </row>
-    <row r="11" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
+      <c r="M10" s="114"/>
+      <c r="N10" s="114"/>
+      <c r="O10" s="114"/>
+      <c r="P10" s="114"/>
+      <c r="Q10" s="114"/>
+      <c r="R10" s="114"/>
+      <c r="S10" s="115"/>
+    </row>
+    <row r="11" spans="1:19" ht="21.95" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="104"/>
-    </row>
-    <row r="12" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="114"/>
+      <c r="Q11" s="114"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="115"/>
+    </row>
+    <row r="12" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="107"/>
-    </row>
-    <row r="13" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="99"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="103"/>
+    </row>
+    <row r="13" spans="1:19" ht="21.95" customHeight="1">
       <c r="A13" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="116" t="s">
+      <c r="D13" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="117"/>
-      <c r="F13" s="117"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="118"/>
-      <c r="P13" s="118"/>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="118"/>
-      <c r="S13" s="119"/>
-    </row>
-    <row r="14" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="107"/>
+      <c r="L13" s="107"/>
+      <c r="M13" s="107"/>
+      <c r="N13" s="107"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
+      <c r="S13" s="116"/>
+    </row>
+    <row r="14" spans="1:19" ht="21.95" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="120" t="s">
+      <c r="D14" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="103"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="103"/>
-      <c r="N14" s="103"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="103"/>
-      <c r="R14" s="103"/>
-      <c r="S14" s="104"/>
-    </row>
-    <row r="15" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="114"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="114"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="114"/>
+      <c r="R14" s="114"/>
+      <c r="S14" s="115"/>
+    </row>
+    <row r="15" spans="1:19" ht="21.95" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="120" t="s">
+      <c r="D15" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="103"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="103"/>
-      <c r="N15" s="103"/>
-      <c r="O15" s="103"/>
-      <c r="P15" s="103"/>
-      <c r="Q15" s="103"/>
-      <c r="R15" s="103"/>
-      <c r="S15" s="104"/>
-    </row>
-    <row r="16" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="114"/>
+      <c r="P15" s="114"/>
+      <c r="Q15" s="114"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="115"/>
+    </row>
+    <row r="16" spans="1:19" ht="21.95" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="120" t="s">
+      <c r="D16" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="103"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
-      <c r="N16" s="103"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="103"/>
-      <c r="S16" s="104"/>
-    </row>
-    <row r="17" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="114"/>
+      <c r="O16" s="114"/>
+      <c r="P16" s="114"/>
+      <c r="Q16" s="114"/>
+      <c r="R16" s="114"/>
+      <c r="S16" s="115"/>
+    </row>
+    <row r="17" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="98"/>
-      <c r="P17" s="95"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="97"/>
-    </row>
-    <row r="18" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="122"/>
+      <c r="N17" s="122"/>
+      <c r="O17" s="124"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="122"/>
+      <c r="R17" s="122"/>
+      <c r="S17" s="123"/>
+    </row>
+    <row r="18" spans="1:19" ht="21.95" customHeight="1">
       <c r="A18" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="108" t="s">
+      <c r="D18" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="103"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109"/>
-      <c r="N18" s="109"/>
-      <c r="O18" s="109"/>
-      <c r="P18" s="109"/>
-      <c r="Q18" s="109"/>
-      <c r="R18" s="109"/>
-      <c r="S18" s="110"/>
-    </row>
-    <row r="19" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="109"/>
+    </row>
+    <row r="19" spans="1:19" ht="21.95" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="23"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="102"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="103"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="103"/>
-      <c r="N19" s="103"/>
-      <c r="O19" s="103"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="103"/>
-      <c r="R19" s="103"/>
-      <c r="S19" s="104"/>
-    </row>
-    <row r="20" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="114"/>
+      <c r="K19" s="114"/>
+      <c r="L19" s="114"/>
+      <c r="M19" s="114"/>
+      <c r="N19" s="114"/>
+      <c r="O19" s="114"/>
+      <c r="P19" s="114"/>
+      <c r="Q19" s="114"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="115"/>
+    </row>
+    <row r="20" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A20" s="25"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="106"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="106"/>
-      <c r="O20" s="106"/>
-      <c r="P20" s="106"/>
-      <c r="Q20" s="106"/>
-      <c r="R20" s="106"/>
-      <c r="S20" s="107"/>
-    </row>
-    <row r="21" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
+      <c r="P20" s="102"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="103"/>
+    </row>
+    <row r="21" spans="1:19" ht="21.95" customHeight="1">
       <c r="A21" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="108" t="s">
+      <c r="D21" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="109"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="109"/>
-      <c r="S21" s="110"/>
-    </row>
-    <row r="22" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="108"/>
+      <c r="P21" s="108"/>
+      <c r="Q21" s="108"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="109"/>
+    </row>
+    <row r="22" spans="1:19" ht="21.95" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="97" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="103"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
-      <c r="K22" s="103"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="103"/>
-      <c r="N22" s="103"/>
-      <c r="O22" s="103"/>
-      <c r="P22" s="103"/>
-      <c r="Q22" s="103"/>
-      <c r="R22" s="103"/>
-      <c r="S22" s="104"/>
-    </row>
-    <row r="23" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="114"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="114"/>
+      <c r="L22" s="114"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="114"/>
+      <c r="O22" s="114"/>
+      <c r="P22" s="114"/>
+      <c r="Q22" s="114"/>
+      <c r="R22" s="114"/>
+      <c r="S22" s="115"/>
+    </row>
+    <row r="23" spans="1:19" ht="21.95" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="103"/>
-      <c r="N23" s="103"/>
-      <c r="O23" s="103"/>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="103"/>
-      <c r="R23" s="103"/>
-      <c r="S23" s="104"/>
-    </row>
-    <row r="24" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="114"/>
+      <c r="J23" s="114"/>
+      <c r="K23" s="114"/>
+      <c r="L23" s="114"/>
+      <c r="M23" s="114"/>
+      <c r="N23" s="114"/>
+      <c r="O23" s="114"/>
+      <c r="P23" s="114"/>
+      <c r="Q23" s="114"/>
+      <c r="R23" s="114"/>
+      <c r="S23" s="115"/>
+    </row>
+    <row r="24" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A24" s="25"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27"/>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="106"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="106"/>
-      <c r="O24" s="106"/>
-      <c r="P24" s="106"/>
-      <c r="Q24" s="106"/>
-      <c r="R24" s="106"/>
-      <c r="S24" s="107"/>
-    </row>
-    <row r="26" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
+      <c r="R24" s="102"/>
+      <c r="S24" s="103"/>
+    </row>
+    <row r="26" spans="1:19" ht="21.95" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="31" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="112" t="s">
+    <row r="28" spans="1:19" s="31" customFormat="1" ht="21.95" customHeight="1" thickBot="1">
+      <c r="A28" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="123" t="s">
+      <c r="B28" s="105"/>
+      <c r="C28" s="105"/>
+      <c r="D28" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="124"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="124"/>
-      <c r="I28" s="124"/>
-      <c r="J28" s="124"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="124"/>
-      <c r="M28" s="124"/>
-      <c r="N28" s="124"/>
-      <c r="O28" s="124"/>
-      <c r="P28" s="125" t="s">
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="111"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="111"/>
+      <c r="P28" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="Q28" s="124"/>
-      <c r="R28" s="124"/>
-      <c r="S28" s="126"/>
-    </row>
-    <row r="29" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="116" t="s">
+      <c r="Q28" s="111"/>
+      <c r="R28" s="111"/>
+      <c r="S28" s="113"/>
+    </row>
+    <row r="29" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A29" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="132"/>
-      <c r="H29" s="132"/>
-      <c r="I29" s="132"/>
-      <c r="J29" s="132"/>
-      <c r="K29" s="132"/>
-      <c r="L29" s="132"/>
-      <c r="M29" s="132"/>
-      <c r="N29" s="132"/>
-      <c r="O29" s="133"/>
-      <c r="P29" s="134"/>
-      <c r="Q29" s="135"/>
-      <c r="R29" s="135"/>
-      <c r="S29" s="136"/>
-    </row>
-    <row r="30" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="120" t="s">
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="138"/>
+      <c r="K29" s="138"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
+      <c r="O29" s="139"/>
+      <c r="P29" s="140"/>
+      <c r="Q29" s="141"/>
+      <c r="R29" s="141"/>
+      <c r="S29" s="142"/>
+    </row>
+    <row r="30" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A30" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="102"/>
-      <c r="C30" s="102"/>
-      <c r="D30" s="127"/>
-      <c r="E30" s="127"/>
-      <c r="F30" s="127"/>
-      <c r="G30" s="127"/>
-      <c r="H30" s="127"/>
-      <c r="I30" s="127"/>
-      <c r="J30" s="127"/>
-      <c r="K30" s="127"/>
-      <c r="L30" s="127"/>
-      <c r="M30" s="127"/>
-      <c r="N30" s="127"/>
-      <c r="O30" s="128"/>
-      <c r="P30" s="129"/>
-      <c r="Q30" s="130"/>
-      <c r="R30" s="130"/>
-      <c r="S30" s="131"/>
-    </row>
-    <row r="31" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="120" t="s">
+      <c r="B30" s="97"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="143"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="143"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="143"/>
+      <c r="J30" s="143"/>
+      <c r="K30" s="143"/>
+      <c r="L30" s="143"/>
+      <c r="M30" s="143"/>
+      <c r="N30" s="143"/>
+      <c r="O30" s="92"/>
+      <c r="P30" s="144"/>
+      <c r="Q30" s="145"/>
+      <c r="R30" s="145"/>
+      <c r="S30" s="146"/>
+    </row>
+    <row r="31" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A31" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="102"/>
-      <c r="C31" s="102"/>
-      <c r="D31" s="127"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
-      <c r="G31" s="127"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="127"/>
-      <c r="J31" s="127"/>
-      <c r="K31" s="127"/>
-      <c r="L31" s="127"/>
-      <c r="M31" s="127"/>
-      <c r="N31" s="127"/>
-      <c r="O31" s="128"/>
-      <c r="P31" s="129"/>
-      <c r="Q31" s="130"/>
-      <c r="R31" s="130"/>
-      <c r="S31" s="131"/>
-    </row>
-    <row r="32" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="120" t="s">
+      <c r="B31" s="97"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="143"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="143"/>
+      <c r="H31" s="143"/>
+      <c r="I31" s="143"/>
+      <c r="J31" s="143"/>
+      <c r="K31" s="143"/>
+      <c r="L31" s="143"/>
+      <c r="M31" s="143"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="144"/>
+      <c r="Q31" s="145"/>
+      <c r="R31" s="145"/>
+      <c r="S31" s="146"/>
+    </row>
+    <row r="32" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A32" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="102"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="127"/>
-      <c r="J32" s="127"/>
-      <c r="K32" s="127"/>
-      <c r="L32" s="127"/>
-      <c r="M32" s="127"/>
-      <c r="N32" s="127"/>
-      <c r="O32" s="128"/>
-      <c r="P32" s="129"/>
-      <c r="Q32" s="130"/>
-      <c r="R32" s="130"/>
-      <c r="S32" s="131"/>
-    </row>
-    <row r="33" spans="1:19" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="120" t="s">
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="143"/>
+      <c r="E32" s="143"/>
+      <c r="F32" s="143"/>
+      <c r="G32" s="143"/>
+      <c r="H32" s="143"/>
+      <c r="I32" s="143"/>
+      <c r="J32" s="143"/>
+      <c r="K32" s="143"/>
+      <c r="L32" s="143"/>
+      <c r="M32" s="143"/>
+      <c r="N32" s="143"/>
+      <c r="O32" s="92"/>
+      <c r="P32" s="144"/>
+      <c r="Q32" s="145"/>
+      <c r="R32" s="145"/>
+      <c r="S32" s="146"/>
+    </row>
+    <row r="33" spans="1:19" ht="21.95" customHeight="1">
+      <c r="A33" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="102"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="127"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="127"/>
-      <c r="H33" s="127"/>
-      <c r="I33" s="127"/>
-      <c r="J33" s="127"/>
-      <c r="K33" s="127"/>
-      <c r="L33" s="127"/>
-      <c r="M33" s="127"/>
-      <c r="N33" s="127"/>
-      <c r="O33" s="128"/>
-      <c r="P33" s="129"/>
-      <c r="Q33" s="130"/>
-      <c r="R33" s="130"/>
-      <c r="S33" s="131"/>
-    </row>
-    <row r="34" spans="1:19" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="122" t="s">
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="143"/>
+      <c r="F33" s="143"/>
+      <c r="G33" s="143"/>
+      <c r="H33" s="143"/>
+      <c r="I33" s="143"/>
+      <c r="J33" s="143"/>
+      <c r="K33" s="143"/>
+      <c r="L33" s="143"/>
+      <c r="M33" s="143"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="92"/>
+      <c r="P33" s="144"/>
+      <c r="Q33" s="145"/>
+      <c r="R33" s="145"/>
+      <c r="S33" s="146"/>
+    </row>
+    <row r="34" spans="1:19" ht="21.95" customHeight="1" thickBot="1">
+      <c r="A34" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="140"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="140"/>
-      <c r="I34" s="140"/>
-      <c r="J34" s="140"/>
-      <c r="K34" s="140"/>
-      <c r="L34" s="140"/>
-      <c r="M34" s="140"/>
-      <c r="N34" s="140"/>
-      <c r="O34" s="141"/>
-      <c r="P34" s="137"/>
-      <c r="Q34" s="138"/>
-      <c r="R34" s="138"/>
-      <c r="S34" s="139"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="147"/>
+      <c r="E34" s="147"/>
+      <c r="F34" s="147"/>
+      <c r="G34" s="147"/>
+      <c r="H34" s="147"/>
+      <c r="I34" s="147"/>
+      <c r="J34" s="147"/>
+      <c r="K34" s="147"/>
+      <c r="L34" s="147"/>
+      <c r="M34" s="147"/>
+      <c r="N34" s="147"/>
+      <c r="O34" s="148"/>
+      <c r="P34" s="149"/>
+      <c r="Q34" s="150"/>
+      <c r="R34" s="150"/>
+      <c r="S34" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="127">
+    <mergeCell ref="P17:S17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="P22:S22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="P23:S23"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="P19:S19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="P13:S13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P15:S15"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="P24:S24"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="P21:S21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="P28:S28"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:S31"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="P30:S30"/>
     <mergeCell ref="P33:S33"/>
     <mergeCell ref="P34:S34"/>
     <mergeCell ref="A32:C32"/>
@@ -4541,109 +4612,6 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="P31:S31"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P29:S29"/>
-    <mergeCell ref="P30:S30"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="P24:S24"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="P21:S21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="P28:S28"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="P15:S15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="P13:S13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="P22:S22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="P23:S23"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="P19:S19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="P20:S20"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="P18:S18"/>
-    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -4659,15 +4627,15 @@
       <selection activeCell="D30" sqref="D30:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="38" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="18" width="6.85546875" style="38" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="38"/>
+    <col min="1" max="1" width="7.75" style="38" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="6.875" style="38" customWidth="1"/>
+    <col min="19" max="16384" width="9.125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="19.5">
       <c r="A1" s="41" t="s">
         <v>65</v>
       </c>
@@ -4689,7 +4657,7 @@
       <c r="Q1" s="40"/>
       <c r="R1" s="40"/>
     </row>
-    <row r="2" spans="1:18" s="37" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="37" customFormat="1" ht="13.5">
       <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
@@ -4701,8 +4669,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="37" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:18" s="39" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="37" customFormat="1" ht="15" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:18" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A4" s="52" t="s">
         <v>66</v>
       </c>
@@ -4712,11 +4680,11 @@
       <c r="C4" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
       <c r="G4" s="53" t="s">
         <v>79</v>
       </c>
@@ -4754,7 +4722,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
       <c r="C5" s="78"/>
@@ -4774,7 +4742,7 @@
       <c r="Q5" s="78"/>
       <c r="R5" s="79"/>
     </row>
-    <row r="6" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="46"/>
       <c r="C6" s="80"/>
@@ -4794,7 +4762,7 @@
       <c r="Q6" s="80"/>
       <c r="R6" s="81"/>
     </row>
-    <row r="7" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="45"/>
       <c r="B7" s="46"/>
       <c r="C7" s="80"/>
@@ -4814,7 +4782,7 @@
       <c r="Q7" s="80"/>
       <c r="R7" s="81"/>
     </row>
-    <row r="8" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="45"/>
       <c r="B8" s="46"/>
       <c r="C8" s="80"/>
@@ -4834,7 +4802,7 @@
       <c r="Q8" s="80"/>
       <c r="R8" s="81"/>
     </row>
-    <row r="9" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="45"/>
       <c r="B9" s="46"/>
       <c r="C9" s="80"/>
@@ -4854,7 +4822,7 @@
       <c r="Q9" s="80"/>
       <c r="R9" s="81"/>
     </row>
-    <row r="10" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="45"/>
       <c r="B10" s="46"/>
       <c r="C10" s="80"/>
@@ -4874,7 +4842,7 @@
       <c r="Q10" s="80"/>
       <c r="R10" s="81"/>
     </row>
-    <row r="11" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="45"/>
       <c r="B11" s="46"/>
       <c r="C11" s="80"/>
@@ -4894,7 +4862,7 @@
       <c r="Q11" s="80"/>
       <c r="R11" s="81"/>
     </row>
-    <row r="12" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="45"/>
       <c r="B12" s="46"/>
       <c r="C12" s="80"/>
@@ -4914,7 +4882,7 @@
       <c r="Q12" s="80"/>
       <c r="R12" s="81"/>
     </row>
-    <row r="13" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="45"/>
       <c r="B13" s="46"/>
       <c r="C13" s="80"/>
@@ -4934,7 +4902,7 @@
       <c r="Q13" s="80"/>
       <c r="R13" s="81"/>
     </row>
-    <row r="14" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="45"/>
       <c r="B14" s="46"/>
       <c r="C14" s="80"/>
@@ -4954,7 +4922,7 @@
       <c r="Q14" s="80"/>
       <c r="R14" s="81"/>
     </row>
-    <row r="15" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="45"/>
       <c r="B15" s="46"/>
       <c r="C15" s="80"/>
@@ -4974,7 +4942,7 @@
       <c r="Q15" s="80"/>
       <c r="R15" s="81"/>
     </row>
-    <row r="16" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="45"/>
       <c r="B16" s="46"/>
       <c r="C16" s="80"/>
@@ -4994,7 +4962,7 @@
       <c r="Q16" s="80"/>
       <c r="R16" s="81"/>
     </row>
-    <row r="17" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="45"/>
       <c r="B17" s="46"/>
       <c r="C17" s="80"/>
@@ -5014,7 +4982,7 @@
       <c r="Q17" s="80"/>
       <c r="R17" s="81"/>
     </row>
-    <row r="18" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="45"/>
       <c r="B18" s="46"/>
       <c r="C18" s="80"/>
@@ -5034,7 +5002,7 @@
       <c r="Q18" s="80"/>
       <c r="R18" s="81"/>
     </row>
-    <row r="19" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="45"/>
       <c r="B19" s="46"/>
       <c r="C19" s="80"/>
@@ -5054,7 +5022,7 @@
       <c r="Q19" s="80"/>
       <c r="R19" s="81"/>
     </row>
-    <row r="20" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="45"/>
       <c r="B20" s="46"/>
       <c r="C20" s="80"/>
@@ -5074,7 +5042,7 @@
       <c r="Q20" s="80"/>
       <c r="R20" s="81"/>
     </row>
-    <row r="21" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="45"/>
       <c r="B21" s="46"/>
       <c r="C21" s="80"/>
@@ -5094,7 +5062,7 @@
       <c r="Q21" s="80"/>
       <c r="R21" s="81"/>
     </row>
-    <row r="22" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="45"/>
       <c r="B22" s="46"/>
       <c r="C22" s="80"/>
@@ -5114,7 +5082,7 @@
       <c r="Q22" s="80"/>
       <c r="R22" s="81"/>
     </row>
-    <row r="23" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="45"/>
       <c r="B23" s="46"/>
       <c r="C23" s="80"/>
@@ -5134,7 +5102,7 @@
       <c r="Q23" s="80"/>
       <c r="R23" s="81"/>
     </row>
-    <row r="24" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="45"/>
       <c r="B24" s="46"/>
       <c r="C24" s="80"/>
@@ -5154,7 +5122,7 @@
       <c r="Q24" s="80"/>
       <c r="R24" s="81"/>
     </row>
-    <row r="25" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="45"/>
       <c r="B25" s="46"/>
       <c r="C25" s="80"/>
@@ -5174,7 +5142,7 @@
       <c r="Q25" s="80"/>
       <c r="R25" s="81"/>
     </row>
-    <row r="26" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="45"/>
       <c r="B26" s="46"/>
       <c r="C26" s="80"/>
@@ -5194,7 +5162,7 @@
       <c r="Q26" s="80"/>
       <c r="R26" s="81"/>
     </row>
-    <row r="27" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="45"/>
       <c r="B27" s="46"/>
       <c r="C27" s="80"/>
@@ -5214,7 +5182,7 @@
       <c r="Q27" s="80"/>
       <c r="R27" s="81"/>
     </row>
-    <row r="28" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" s="37" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="47"/>
       <c r="B28" s="48"/>
       <c r="C28" s="82"/>
@@ -5234,19 +5202,19 @@
       <c r="Q28" s="82"/>
       <c r="R28" s="83"/>
     </row>
-    <row r="29" spans="1:18" s="37" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="142" t="s">
+    <row r="29" spans="1:18" s="37" customFormat="1" ht="25.5">
+      <c r="A29" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="143"/>
+      <c r="B29" s="129"/>
       <c r="C29" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="150" t="s">
+      <c r="D29" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
       <c r="G29" s="49" t="s">
         <v>79</v>
       </c>
@@ -5284,13 +5252,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="37" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="144"/>
-      <c r="B30" s="145"/>
+    <row r="30" spans="1:18" s="37" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A30" s="130"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="84"/>
-      <c r="D30" s="147"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="149"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="135"/>
       <c r="G30" s="84"/>
       <c r="H30" s="84"/>
       <c r="I30" s="84"/>

</xml_diff>